<commit_message>
Graph now dynamically scales, picture updates are cleaner
</commit_message>
<xml_diff>
--- a/scratch.xlsx
+++ b/scratch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="4200" windowHeight="1290"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -342,10 +342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D3:H27"/>
+  <dimension ref="D3:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H27"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -361,8 +361,8 @@
         <v>0</v>
       </c>
       <c r="H3" t="str">
-        <f>"output.append([" &amp;D3 &amp; ", " &amp; E3 &amp; ", " &amp; F3 &amp; "])"</f>
-        <v>output.append([0, 27.3388888888889, 0])</v>
+        <f>"sun.append(" &amp; F3 &amp; ")"</f>
+        <v>sun.append(0)</v>
       </c>
     </row>
     <row r="4" spans="4:8">
@@ -376,8 +376,8 @@
         <v>0</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H4:H27" si="0">"output.append([" &amp;D4 &amp; ", " &amp; E4 &amp; ", " &amp; F4 &amp; "])"</f>
-        <v>output.append([0.0416666666666667, 24.6777777777778, 0])</v>
+        <f t="shared" ref="H4:H27" si="0">"sun.append(" &amp; F4 &amp; ")"</f>
+        <v>sun.append(0)</v>
       </c>
     </row>
     <row r="5" spans="4:8">
@@ -392,7 +392,7 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.0833333333333333, 22.0166666666667, 0])</v>
+        <v>sun.append(0)</v>
       </c>
     </row>
     <row r="6" spans="4:8">
@@ -407,7 +407,7 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.125, 19.3555555555556, 0])</v>
+        <v>sun.append(0)</v>
       </c>
     </row>
     <row r="7" spans="4:8">
@@ -422,7 +422,7 @@
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.166666666666667, 16.6944444444444, 0])</v>
+        <v>sun.append(0)</v>
       </c>
     </row>
     <row r="8" spans="4:8">
@@ -437,7 +437,7 @@
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.208333333333333, 14.0333333333333, 0])</v>
+        <v>sun.append(0)</v>
       </c>
     </row>
     <row r="9" spans="4:8">
@@ -452,7 +452,7 @@
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.25, 11.3722222222222, 0])</v>
+        <v>sun.append(0)</v>
       </c>
     </row>
     <row r="10" spans="4:8">
@@ -467,7 +467,7 @@
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.291666666666667, 10.2219500964689, 1.34417231869112])</v>
+        <v>sun.append(1.34417231869112)</v>
       </c>
     </row>
     <row r="11" spans="4:8">
@@ -482,7 +482,7 @@
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.333333333333333, 10.1375278343533, 2.63668884899547])</v>
+        <v>sun.append(2.63668884899547)</v>
       </c>
     </row>
     <row r="12" spans="4:8">
@@ -497,7 +497,7 @@
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.375, 11.2442956287472, 3.82787890550506])</v>
+        <v>sun.append(3.82787890550506)</v>
       </c>
     </row>
     <row r="13" spans="4:8">
@@ -512,7 +512,7 @@
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.416666666666667, 13.3951502400114, 4.87196572237531])</v>
+        <v>sun.append(4.87196572237531)</v>
       </c>
     </row>
     <row r="14" spans="4:8">
@@ -527,7 +527,7 @@
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.458333333333333, 16.4028647576648, 5.72882562876454])</v>
+        <v>sun.append(5.72882562876454)</v>
       </c>
     </row>
     <row r="15" spans="4:8">
@@ -542,7 +542,7 @@
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.5, 20.0472836255565, 6.36552997900277])</v>
+        <v>sun.append(6.36552997900277)</v>
       </c>
     </row>
     <row r="16" spans="4:8">
@@ -557,7 +557,7 @@
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.541666666666667, 24.0837830964236, 6.75761058197826])</v>
+        <v>sun.append(6.75761058197826)</v>
       </c>
     </row>
     <row r="17" spans="4:8">
@@ -572,7 +572,7 @@
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.583333333333333, 28.2526719853125, 6.89])</v>
+        <v>sun.append(6.89)</v>
       </c>
     </row>
     <row r="18" spans="4:8">
@@ -587,7 +587,7 @@
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.625, 32.2891714561797, 6.75761058197826])</v>
+        <v>sun.append(6.75761058197826)</v>
       </c>
     </row>
     <row r="19" spans="4:8">
@@ -602,7 +602,7 @@
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.666666666666667, 35.9335903240713, 6.36552997900277])</v>
+        <v>sun.append(6.36552997900277)</v>
       </c>
     </row>
     <row r="20" spans="4:8">
@@ -617,7 +617,7 @@
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.708333333333333, 38.9413048417248, 5.72882562876454])</v>
+        <v>sun.append(5.72882562876454)</v>
       </c>
     </row>
     <row r="21" spans="4:8">
@@ -632,7 +632,7 @@
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.75, 41.092159452989, 4.87196572237531])</v>
+        <v>sun.append(4.87196572237531)</v>
       </c>
     </row>
     <row r="22" spans="4:8">
@@ -647,7 +647,7 @@
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.791666666666667, 42.1989272473829, 3.82787890550506])</v>
+        <v>sun.append(3.82787890550506)</v>
       </c>
     </row>
     <row r="23" spans="4:8">
@@ -662,7 +662,7 @@
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.833333333333333, 41.8145049852673, 2.63668884899547])</v>
+        <v>sun.append(2.63668884899547)</v>
       </c>
     </row>
     <row r="24" spans="4:8">
@@ -677,7 +677,7 @@
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.875, 37.9375661928473, 1.34417231869113])</v>
+        <v>sun.append(1.34417231869113)</v>
       </c>
     </row>
     <row r="25" spans="4:8">
@@ -692,7 +692,7 @@
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.916666666666667, 34.7164550817362, 8.44127285432039E-16])</v>
+        <v>sun.append(8.44127285432039E-16)</v>
       </c>
     </row>
     <row r="26" spans="4:8">
@@ -707,7 +707,7 @@
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([0.958333333333333, 32.0553439706251, 0])</v>
+        <v>sun.append(0)</v>
       </c>
     </row>
     <row r="27" spans="4:8">
@@ -722,7 +722,13 @@
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
-        <v>output.append([1, 29.3942328595139, 0])</v>
+        <v>sun.append(0)</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8">
+      <c r="F31">
+        <f>455/250</f>
+        <v>1.82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>